<commit_message>
Update doku / workflow / WebApp Installation
</commit_message>
<xml_diff>
--- a/Vorlage Betriebsdokumentation.xlsx
+++ b/Vorlage Betriebsdokumentation.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE7916C8-D444-4BC5-A84B-BBCDBDA87FE5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C77FB3B5-E75D-4488-8D92-E42D5DC35DE3}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="758" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="758" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjektOrga" sheetId="19" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="54">
   <si>
     <t>Monitoring</t>
   </si>
@@ -162,6 +162,39 @@
   </si>
   <si>
     <t>(Nur der Projektleiter des Kunden erhält Zugang zu dieser, nicht alle Projektmitarbeiter)</t>
+  </si>
+  <si>
+    <t>Administratorenmappe</t>
+  </si>
+  <si>
+    <t>Steuerungsfunktionen (lösen Stored Procedures aus)</t>
+  </si>
+  <si>
+    <t>Process Log Ansicht</t>
+  </si>
+  <si>
+    <t>Fehlerreport</t>
+  </si>
+  <si>
+    <t>Usermappe</t>
+  </si>
+  <si>
+    <t>Inhaltsverzeichnis</t>
+  </si>
+  <si>
+    <t>Eventauswertung</t>
+  </si>
+  <si>
+    <t>Alle Reports nutzen Benutzerrechte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reports kann basieren auf </t>
+  </si>
+  <si>
+    <t>direkter SQL Verbindung</t>
+  </si>
+  <si>
+    <t>Azure Webservice Verbindung per PowerQuery</t>
   </si>
 </sst>
 </file>
@@ -35787,7 +35820,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD7A2A25-57D6-42FC-813F-54EC03E0F65D}">
   <dimension ref="B1:B2"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
@@ -35926,10 +35959,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="B1:U10"/>
+  <dimension ref="B1:U65"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36001,6 +36034,71 @@
       </c>
       <c r="U10" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="48" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O48" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="15:16" x14ac:dyDescent="0.25">
+      <c r="P49" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="15:16" x14ac:dyDescent="0.25">
+      <c r="P51" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="15:16" x14ac:dyDescent="0.25">
+      <c r="P52" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="54" spans="15:16" x14ac:dyDescent="0.25">
+      <c r="O54" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="55" spans="15:16" x14ac:dyDescent="0.25">
+      <c r="P55" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="56" spans="15:16" x14ac:dyDescent="0.25">
+      <c r="P56" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="57" spans="15:16" x14ac:dyDescent="0.25">
+      <c r="P57" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="58" spans="15:16" x14ac:dyDescent="0.25">
+      <c r="P58" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="61" spans="15:16" x14ac:dyDescent="0.25">
+      <c r="O61" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="63" spans="15:16" x14ac:dyDescent="0.25">
+      <c r="O63" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="64" spans="15:16" x14ac:dyDescent="0.25">
+      <c r="P64" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="65" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P65" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>